<commit_message>
Subtree of another tree shortcut
</commit_message>
<xml_diff>
--- a/Leetcode learnings.xlsx
+++ b/Leetcode learnings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amey/Desktop/repos/Leetcode-Learnings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336B2B0D-A3C0-CD4D-8A2E-8E1E0043D63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA517EB-C8F5-B94C-BBB4-BE7A9074B0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16900" activeTab="2" xr2:uid="{C2ABFAF5-9768-A849-993B-3087B2A527A2}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Interesting patterns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="254">
   <si>
     <t> Two Sum</t>
   </si>
@@ -887,6 +886,19 @@
   <si>
     <t>1. Iterate from the start, and store the intermediate results
 2. Use this results for the next iteration</t>
+  </si>
+  <si>
+    <t>Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t>Prefix traversal</t>
+  </si>
+  <si>
+    <t>1. Can compare with same tree
+2. Some traversal might be the same</t>
+  </si>
+  <si>
+    <t>1. Updating or tweaking the traversal to get the desired result, better than comparing the tree over and over again</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1012,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1056,6 +1068,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2354,10 +2369,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602BD977-30B7-A347-8E5A-13E9B558F709}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2578,6 +2593,20 @@
       </c>
       <c r="D16" s="5" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2597,6 +2626,7 @@
     <hyperlink ref="A14" r:id="rId8" display="https://leetcode.com/problems/top-k-frequent-elements/" xr:uid="{D903E004-602B-E546-A72D-8F3D8F8CCEA5}"/>
     <hyperlink ref="A15" r:id="rId9" display="https://leetcode.com/problems/smallest-string-with-swaps/" xr:uid="{B523E1BA-017D-0647-9B38-2D7E434DC974}"/>
     <hyperlink ref="A16" r:id="rId10" display="https://leetcode.com/problems/word-break/" xr:uid="{89A07081-07F9-DB47-9693-34CE71AD1BDB}"/>
+    <hyperlink ref="A17" r:id="rId11" display="https://leetcode.com/problems/subtree-of-another-tree/" xr:uid="{90E8EAB5-A462-4847-BA4F-0DCFDBA77D52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>